<commit_message>
Prepare to integrate SDK
</commit_message>
<xml_diff>
--- a/Assets/Scripts/PVPSdk/错误码.xlsx
+++ b/Assets/Scripts/PVPSdk/错误码.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22810"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16300" tabRatio="500"/>
+    <workbookView xWindow="7760" yWindow="0" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="错误码" sheetId="1" r:id="rId1"/>
@@ -19,102 +19,150 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>错误名称</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>描述</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SUCCESS</t>
+  </si>
+  <si>
+    <t>UNKNOWN</t>
+  </si>
+  <si>
+    <t>SERVICE_ERROR</t>
+  </si>
+  <si>
+    <t>METHOD_UNKNOWN</t>
+  </si>
+  <si>
+    <t>调用的方法不存在</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TOO_MANY_CALLS</t>
+  </si>
+  <si>
+    <t>BAD_IP</t>
+  </si>
+  <si>
+    <t>DB_ERROR</t>
+  </si>
+  <si>
+    <t>IS_CHEAT</t>
+  </si>
+  <si>
+    <t>用户作弊</t>
+  </si>
+  <si>
+    <t>NEED_LOGIN</t>
+  </si>
+  <si>
+    <t>ACCOUNT_OR_PASSWORD_ERROR</t>
+  </si>
+  <si>
+    <t>DATA_ERROR</t>
+  </si>
+  <si>
+    <t>CP_LIMIT</t>
+  </si>
+  <si>
+    <t>VERSION_IS_OLD</t>
+  </si>
+  <si>
+    <t>版本过旧</t>
+  </si>
+  <si>
+    <t>APP_NOT_EXIST</t>
+  </si>
+  <si>
+    <t>应用不存在</t>
+  </si>
+  <si>
+    <t>PARAM_ERROR</t>
+  </si>
+  <si>
+    <t>PARAM_TOKEN</t>
+  </si>
+  <si>
+    <t>INVALID_MOBILE</t>
+  </si>
+  <si>
+    <t>INVALID_EMAIL</t>
+  </si>
+  <si>
+    <t>CAN_NOT_REQUEST</t>
+  </si>
+  <si>
+    <t>USER_NO_EXIST</t>
+  </si>
+  <si>
+    <t>USER_PASSWORD_ERROR</t>
+  </si>
+  <si>
+    <t>USER_ACCOUNT_REPEATED</t>
+  </si>
+  <si>
+    <t>USER_STATE_NOT_NORMAL</t>
+  </si>
+  <si>
+    <t>USER_PASSWORD_FORMAT_ERROR</t>
+  </si>
+  <si>
+    <t>USER_LOGIN_TYPE_ERROR</t>
+  </si>
+  <si>
+    <t>USER_LOGIN_FACEBOOK_ACCESS_TOKEN_ERROR</t>
+  </si>
+  <si>
+    <t>USER_REGISTER_FAILED</t>
+  </si>
+  <si>
+    <t>ROOM_NOT_EXIST</t>
+  </si>
+  <si>
+    <t>ROOM_CACHE_MESSAGE_NUMBER_NOT_EXIST</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROOM_NOT_IN_ROOM_ERROR</t>
+  </si>
+  <si>
+    <t>ROOM_TARGET_UID_NOT_IN_ROOM_ERROR</t>
+  </si>
+  <si>
+    <t>ROOM_NO_MORE_ROOM_ERROR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ROOM_UPDATE_ROOM_CHECK_DATA_NOT_PASS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESPONSE_TIME_OUT</t>
+  </si>
+  <si>
     <t>编码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SUCCESS</t>
-  </si>
-  <si>
     <t>成功</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UNKNOWN</t>
-  </si>
-  <si>
     <t>错误未知</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>SERVICE_ERROR</t>
-  </si>
-  <si>
     <t>服务器错误</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>METHOD_UNKNOWN</t>
-  </si>
-  <si>
-    <t>调用的方法不存在</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TOO_MANY_CALLS</t>
-  </si>
-  <si>
-    <t>BAD_IP</t>
-  </si>
-  <si>
-    <t>DB_ERROR</t>
-  </si>
-  <si>
-    <t>IS_CHEAT</t>
-  </si>
-  <si>
-    <t>用户作弊</t>
-  </si>
-  <si>
-    <t>NEED_LOGIN</t>
-  </si>
-  <si>
-    <t>ACCOUNT_OR_PASSWORD_ERROR</t>
-  </si>
-  <si>
-    <t>DATA_ERROR</t>
-  </si>
-  <si>
-    <t>CP_LIMIT</t>
-  </si>
-  <si>
-    <t>VERSION_IS_OLD</t>
-  </si>
-  <si>
-    <t>版本过旧</t>
-  </si>
-  <si>
-    <t>APP_NOT_EXIST</t>
-  </si>
-  <si>
-    <t>应用不存在</t>
-  </si>
-  <si>
-    <t>PARAM_ERROR</t>
-  </si>
-  <si>
-    <t>PARAM_TOKEN</t>
-  </si>
-  <si>
-    <t>INVALID_MOBILE</t>
-  </si>
-  <si>
-    <t>INVALID_EMAIL</t>
-  </si>
-  <si>
-    <t>CAN_NOT_REQUEST</t>
-  </si>
-  <si>
     <t>LOBBY_GET_LIST_ERROR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -127,60 +175,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>USER_NO_EXIST</t>
-  </si>
-  <si>
-    <t>USER_PASSWORD_ERROR</t>
-  </si>
-  <si>
-    <t>USER_ACCOUNT_REPEATED</t>
-  </si>
-  <si>
-    <t>USER_STATE_NOT_NORMAL</t>
-  </si>
-  <si>
-    <t>USER_PASSWORD_FORMAT_ERROR</t>
-  </si>
-  <si>
-    <t>USER_LOGIN_TYPE_ERROR</t>
-  </si>
-  <si>
-    <t>USER_LOGIN_FACEBOOK_ACCESS_TOKEN_ERROR</t>
-  </si>
-  <si>
-    <t>USER_REGISTER_FAILED</t>
-  </si>
-  <si>
-    <t>ROOM_NOT_EXIST</t>
-  </si>
-  <si>
-    <t>ROOM_CACHE_MESSAGE_NUMBER_NOT_EXIST</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>房间用户缓存数据不存在</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ROOM_NOT_IN_ROOM_ERROR</t>
-  </si>
-  <si>
-    <t>ROOM_TARGET_UID_NOT_IN_ROOM_ERROR</t>
-  </si>
-  <si>
-    <t>ROOM_NO_MORE_ROOM_ERROR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ROOM_UPDATE_MEMBER_CHECK_DATA_NOT_PASS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ROOM_UPDATE_ROOM_CHECK_DATA_NOT_PASS</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RESPONSE_TIME_OUT</t>
+    <t>APPUSER_CHECK_NOT_PASS</t>
   </si>
 </sst>
 </file>
@@ -234,8 +237,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="普通" xfId="0" builtinId="0"/>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F24" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -585,59 +588,59 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>4</v>
@@ -645,7 +648,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>5</v>
@@ -653,7 +656,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>6</v>
@@ -661,18 +664,18 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B10" s="1">
         <v>8</v>
@@ -680,7 +683,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>9</v>
@@ -688,7 +691,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
         <v>11</v>
@@ -696,7 +699,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
         <v>12</v>
@@ -704,29 +707,29 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1">
         <v>100</v>
@@ -734,7 +737,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1">
         <v>102</v>
@@ -742,7 +745,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B19" s="1">
         <v>103</v>
@@ -750,7 +753,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B20" s="1">
         <v>104</v>
@@ -758,7 +761,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1">
         <v>106</v>
@@ -766,7 +769,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="B23" s="1">
         <v>200</v>
@@ -774,22 +777,22 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B24" s="1">
         <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:3">
-      <c r="A26" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="A26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1">
         <v>10001</v>
@@ -797,7 +800,7 @@
     </row>
     <row r="28" spans="1:3">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1">
         <v>10002</v>
@@ -805,7 +808,7 @@
     </row>
     <row r="29" spans="1:3">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B29" s="1">
         <v>10003</v>
@@ -813,7 +816,7 @@
     </row>
     <row r="30" spans="1:3">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1">
         <v>10004</v>
@@ -821,7 +824,7 @@
     </row>
     <row r="31" spans="1:3">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1">
         <v>10005</v>
@@ -829,7 +832,7 @@
     </row>
     <row r="32" spans="1:3">
       <c r="A32" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1">
         <v>10006</v>
@@ -837,7 +840,7 @@
     </row>
     <row r="33" spans="1:3">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="B33" s="1">
         <v>10007</v>
@@ -845,7 +848,7 @@
     </row>
     <row r="34" spans="1:3">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B34" s="1">
         <v>10008</v>
@@ -853,7 +856,7 @@
     </row>
     <row r="36" spans="1:3">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B36" s="1">
         <v>11001</v>
@@ -861,18 +864,18 @@
     </row>
     <row r="37" spans="1:3">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1">
         <v>11002</v>
       </c>
       <c r="C37" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="B38" s="1">
         <v>11003</v>
@@ -880,7 +883,7 @@
     </row>
     <row r="39" spans="1:3">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="B39" s="1">
         <v>11004</v>
@@ -888,7 +891,7 @@
     </row>
     <row r="40" spans="1:3">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1">
         <v>11005</v>
@@ -896,7 +899,7 @@
     </row>
     <row r="41" spans="1:3">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B41" s="1">
         <v>11006</v>
@@ -904,17 +907,25 @@
     </row>
     <row r="42" spans="1:3">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B42" s="1">
         <v>11007</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B45" s="1">
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="1">
+        <v>12001</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B46" s="1">
         <v>90000</v>
       </c>
     </row>

</xml_diff>